<commit_message>
Update Weekly Report 26/05/2023
</commit_message>
<xml_diff>
--- a/WeeklyReport/RVC_AUTOSARCP_MCAL_Weekly_Report_26052023.xlsx
+++ b/WeeklyReport/RVC_AUTOSARCP_MCAL_Weekly_Report_26052023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\tminhduy\Desktop\WeeklyReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D722A95A-1932-4663-9E2A-78381A955DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAABE67-EE4E-435E-9743-0A5D126ED3F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -836,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1244,7 +1244,7 @@
         <v>12</v>
       </c>
       <c r="G22" s="37">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="H22" s="33" t="s">
         <v>9</v>

</xml_diff>